<commit_message>
Finalized Program: calcGreeks final and hedge pressure code are good for calculating the hedge pressure at 30 min before the stock market closes these code will allow me to test whether hedge pressure can predicat movement in the final 30 min and if it also correlates with reversals the following morning
Next Steps:
I need to figure out how to get the code to run every day for at 30 before stock market close
I need to figure out how to record the hedge pressure readings and record return in the final 30 min and return in the first 30 min of open
If I can get a lot of dat I could use it o train a machine learning that takes the hedge pressure input and other factors to predict opening 30 whether up or down
</commit_message>
<xml_diff>
--- a/calls_dol_gammas.xlsx
+++ b/calls_dol_gammas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPY 2023-06-28" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SPY 2023-06-29" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SPY230628C00380000</t>
+          <t>SPY230629C00380000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -549,25 +549,25 @@
         <v>380</v>
       </c>
       <c r="E2" t="n">
-        <v>53.81</v>
+        <v>55.9</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>55.29</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>55.54</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>2.3199997</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>4.329973</v>
       </c>
       <c r="J2" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L2" t="n">
         <v>1e-05</v>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.021</v>
+        <v>0.01</v>
       </c>
       <c r="T2" t="n">
         <v>-0.055</v>
@@ -610,7 +610,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SPY230628C00390000</t>
+          <t>SPY230629C00390000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -618,25 +618,25 @@
         <v>390</v>
       </c>
       <c r="E3" t="n">
-        <v>43.49</v>
+        <v>44.91</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>45.3</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>45.55</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>-1.7999992</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>-3.853563</v>
       </c>
       <c r="J3" t="n">
-        <v>553</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
         <v>1e-05</v>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.021</v>
+        <v>0.011</v>
       </c>
       <c r="T3" t="n">
         <v>-0.056</v>
@@ -679,7 +679,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SPY230628C00400000</t>
+          <t>SPY230629C00400000</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -687,25 +687,25 @@
         <v>400</v>
       </c>
       <c r="E4" t="n">
-        <v>37.8</v>
+        <v>35.67</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>35.26</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>35.55</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>3.709999</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>11.608258</v>
       </c>
       <c r="J4" t="n">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
         <v>1e-05</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0.022</v>
+        <v>0.011</v>
       </c>
       <c r="T4" t="n">
         <v>-0.058</v>
@@ -748,32 +748,34 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SPY230628C00408000</t>
+          <t>SPY230629C00410000</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E5" t="n">
-        <v>26.61</v>
+        <v>25.59</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>25.3</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>25.55</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>2.8099995</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>12.335379</v>
       </c>
       <c r="J5" t="n">
-        <v>7</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="K5" t="n">
+        <v>17</v>
+      </c>
       <c r="L5" t="n">
         <v>1e-05</v>
       </c>
@@ -800,12 +802,14 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0.022</v>
+        <v>0.011</v>
       </c>
       <c r="T5" t="n">
         <v>-0.059</v>
       </c>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -813,33 +817,33 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SPY230628C00410000</t>
+          <t>SPY230629C00420000</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="E6" t="n">
-        <v>24.2</v>
+        <v>15.85</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>15.39</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>15.65</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-0.6900005299999999</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>-4.171708</v>
       </c>
       <c r="J6" t="n">
-        <v>34</v>
+        <v>155</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="L6" t="n">
         <v>1e-05</v>
@@ -867,10 +871,10 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0.022</v>
+        <v>0.012</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.059</v>
+        <v>-0.06</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -882,32 +886,34 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SPY230628C00414000</t>
+          <t>SPY230629C00424000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="E7" t="n">
-        <v>19.3</v>
+        <v>11.75</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>11.34</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>11.56</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>-1.0299997</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>-8.059464999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
+        <v>155</v>
+      </c>
+      <c r="K7" t="n">
+        <v>49</v>
+      </c>
       <c r="L7" t="n">
         <v>1e-05</v>
       </c>
@@ -934,12 +940,14 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="U7" t="inlineStr"/>
+        <v>-0.061</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -947,32 +955,34 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SPY230628C00418000</t>
+          <t>SPY230629C00426000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="E8" t="n">
-        <v>15.56</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>9.42</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>9.65</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>-7.2886295</v>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
+        <v>101</v>
+      </c>
+      <c r="K8" t="n">
+        <v>20</v>
+      </c>
       <c r="L8" t="n">
         <v>1e-05</v>
       </c>
@@ -999,12 +1009,14 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="U8" t="inlineStr"/>
+        <v>-0.061</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1012,33 +1024,33 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SPY230628C00420000</t>
+          <t>SPY230629C00428000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="E9" t="n">
-        <v>13.3</v>
+        <v>7.61</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>7.35</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>7.57</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>-1.3200002</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>-14.781636</v>
       </c>
       <c r="J9" t="n">
-        <v>1215</v>
+        <v>68</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="L9" t="n">
         <v>1e-05</v>
@@ -1066,10 +1078,10 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.06</v>
+        <v>-0.062</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
@@ -1081,32 +1093,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SPY230628C00422000</t>
+          <t>SPY230629C00429000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="E10" t="n">
-        <v>12.67</v>
+        <v>6.48</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>6.37</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>6.61</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>-10.373444</v>
       </c>
       <c r="J10" t="n">
-        <v>70</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
+        <v>82</v>
+      </c>
+      <c r="K10" t="n">
+        <v>122</v>
+      </c>
       <c r="L10" t="n">
         <v>1e-05</v>
       </c>
@@ -1133,12 +1147,14 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="U10" t="inlineStr"/>
+        <v>-0.062</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1146,32 +1162,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SPY230628C00424000</t>
+          <t>SPY230629C00430000</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E11" t="n">
-        <v>9.34</v>
+        <v>5.59</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>5.39</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>-0.7100000400000001</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>-11.269841</v>
       </c>
       <c r="J11" t="n">
-        <v>4</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
+        <v>434</v>
+      </c>
+      <c r="K11" t="n">
+        <v>894</v>
+      </c>
       <c r="L11" t="n">
         <v>1e-05</v>
       </c>
@@ -1198,12 +1216,14 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.061</v>
-      </c>
-      <c r="U11" t="inlineStr"/>
+        <v>-0.062</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1211,33 +1231,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SPY230628C00426000</t>
+          <t>SPY230629C00431000</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="E12" t="n">
-        <v>7.62</v>
+        <v>4.54</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>4.36</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>4.59</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>-1.5100002</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>-24.958681</v>
       </c>
       <c r="J12" t="n">
-        <v>8</v>
+        <v>1102</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>2429</v>
       </c>
       <c r="L12" t="n">
         <v>1e-05</v>
@@ -1265,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.061</v>
+        <v>-0.062</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -1280,33 +1300,33 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SPY230628C00427000</t>
+          <t>SPY230629C00432000</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E13" t="n">
-        <v>7.19</v>
+        <v>3.65</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>3.48</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>3.64</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>-0.7999997</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>-17.977522</v>
       </c>
       <c r="J13" t="n">
-        <v>71</v>
+        <v>1185</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>2962</v>
       </c>
       <c r="L13" t="n">
         <v>1e-05</v>
@@ -1334,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.061</v>
+        <v>-0.062</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1349,33 +1369,33 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SPY230628C00428000</t>
+          <t>SPY230629C00433000</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="E14" t="n">
-        <v>6.11</v>
+        <v>2.78</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>2.68</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>2.71</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-0.77</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>-21.690142</v>
       </c>
       <c r="J14" t="n">
-        <v>104</v>
+        <v>5659</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>3625</v>
       </c>
       <c r="L14" t="n">
         <v>1e-05</v>
@@ -1403,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0.023</v>
+        <v>0.012</v>
       </c>
       <c r="T14" t="n">
         <v>-0.062</v>
@@ -1418,36 +1438,36 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SPY230628C00429000</t>
+          <t>SPY230629C00434000</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="E15" t="n">
-        <v>4.95</v>
+        <v>2.03</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>-0.77</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>-27.5</v>
       </c>
       <c r="J15" t="n">
-        <v>106</v>
+        <v>24408</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>4854</v>
       </c>
       <c r="L15" t="n">
-        <v>1e-05</v>
+        <v>0.06714800048828126</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
@@ -1463,22 +1483,22 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>0.878</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>0.132</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="S15" t="n">
-        <v>0.024</v>
+        <v>0.01</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.062</v>
+        <v>-0.21</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>27918428.16049805</v>
       </c>
     </row>
     <row r="16">
@@ -1487,36 +1507,36 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SPY230628C00430000</t>
+          <t>SPY230629C00435000</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="E16" t="n">
-        <v>4.06</v>
+        <v>1.42</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>-0.7200001499999999</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>-33.644863</v>
       </c>
       <c r="J16" t="n">
-        <v>163</v>
+        <v>101637</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>7759</v>
       </c>
       <c r="L16" t="n">
-        <v>1e-05</v>
+        <v>0.07715766601562501</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -1532,22 +1552,22 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>1</v>
+        <v>0.672</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>0.205</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>0.082</v>
       </c>
       <c r="S16" t="n">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.062</v>
+        <v>-0.36</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
+        <v>69306963.70370482</v>
       </c>
     </row>
     <row r="17">
@@ -1556,39 +1576,39 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SPY230628C00431000</t>
+          <t>SPY230629C00436000</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="E17" t="n">
-        <v>3.35</v>
+        <v>0.91</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>-0.6499999</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>-41.666664</v>
       </c>
       <c r="J17" t="n">
-        <v>326</v>
+        <v>199597</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>7028</v>
       </c>
       <c r="L17" t="n">
-        <v>1e-05</v>
+        <v>0.07996525512695313</v>
       </c>
       <c r="M17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1601,22 +1621,22 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>0.452</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>0.217</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="S17" t="n">
-        <v>0.024</v>
+        <v>0.005</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.062</v>
+        <v>-0.389</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
+        <v>66452105.64436036</v>
       </c>
     </row>
     <row r="18">
@@ -1625,39 +1645,39 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SPY230628C00432000</t>
+          <t>SPY230629C00437000</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="E18" t="n">
-        <v>2.64</v>
+        <v>0.54</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>-0.57</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>-51.35135</v>
       </c>
       <c r="J18" t="n">
-        <v>4525</v>
+        <v>134524</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>4017</v>
       </c>
       <c r="L18" t="n">
-        <v>1e-05</v>
+        <v>0.081063876953125</v>
       </c>
       <c r="M18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -1670,22 +1690,22 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>1</v>
+        <v>0.255</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>0.174</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>0.073</v>
       </c>
       <c r="S18" t="n">
-        <v>0.024</v>
+        <v>0.003</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.062</v>
+        <v>-0.313</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>30455682.77054444</v>
       </c>
     </row>
     <row r="19">
@@ -1694,39 +1714,39 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SPY230628C00433000</t>
+          <t>SPY230629C00438000</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="E19" t="n">
-        <v>2.04</v>
+        <v>0.29</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.29</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>-0.45000002</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>-60.81081</v>
       </c>
       <c r="J19" t="n">
-        <v>8980</v>
+        <v>63264</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>4199</v>
       </c>
       <c r="L19" t="n">
-        <v>1e-05</v>
+        <v>0.08326112060546878</v>
       </c>
       <c r="M19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -1739,22 +1759,22 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>1</v>
+        <v>0.122</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>0.107</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="S19" t="n">
-        <v>0.024</v>
+        <v>0.001</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.062</v>
+        <v>-0.2</v>
       </c>
       <c r="U19" t="n">
-        <v>0</v>
+        <v>19577034.78467407</v>
       </c>
     </row>
     <row r="20">
@@ -1763,36 +1783,36 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SPY230628C00434000</t>
+          <t>SPY230629C00439000</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="E20" t="n">
-        <v>1.53</v>
+        <v>0.16</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>-0.34</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>-68</v>
       </c>
       <c r="J20" t="n">
-        <v>13902</v>
+        <v>51433</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>2929</v>
       </c>
       <c r="L20" t="n">
-        <v>0.007822421875000001</v>
+        <v>0.08374939697265626</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
@@ -1808,22 +1828,22 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>0.004</v>
+        <v>0.047</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.048</v>
+        <v>0.051</v>
       </c>
       <c r="R20" t="n">
-        <v>0.004</v>
+        <v>0.022</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.001</v>
+        <v>-0.096</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>6508888.140032959</v>
       </c>
     </row>
     <row r="21">
@@ -1832,36 +1852,36 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SPY230628C00435000</t>
+          <t>SPY230629C00440000</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E21" t="n">
-        <v>1.11</v>
+        <v>0.08</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>-0.23</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-74.19355</v>
       </c>
       <c r="J21" t="n">
-        <v>18622</v>
+        <v>75854</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>8585</v>
       </c>
       <c r="L21" t="n">
-        <v>0.01563484375</v>
+        <v>0.08692319335937501</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -1877,22 +1897,22 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>0.017</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.003</v>
+        <v>0.021</v>
       </c>
       <c r="R21" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>-0.043</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>7855554.651763918</v>
       </c>
     </row>
     <row r="22">
@@ -1901,36 +1921,36 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SPY230628C00436000</t>
+          <t>SPY230629C00441000</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>-0.13000001</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>-72.22223</v>
       </c>
       <c r="J22" t="n">
-        <v>8612</v>
+        <v>23319</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>2061</v>
       </c>
       <c r="L22" t="n">
-        <v>0.01563484375</v>
+        <v>0.09327078613281251</v>
       </c>
       <c r="M22" t="b">
         <v>0</v>
@@ -1946,22 +1966,22 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>-0.022</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>898039.1123657227</v>
       </c>
     </row>
     <row r="23">
@@ -1970,36 +1990,36 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SPY230628C00437000</t>
+          <t>SPY230629C00442000</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="E23" t="n">
-        <v>0.55</v>
+        <v>0.02</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>-0.09</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>-81.818184</v>
       </c>
       <c r="J23" t="n">
-        <v>6878</v>
+        <v>9819</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>3510</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0312596875</v>
+        <v>0.098641826171875</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -2015,22 +2035,22 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>-0.011</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>611764.6354980469</v>
       </c>
     </row>
     <row r="24">
@@ -2039,36 +2059,36 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SPY230628C00438000</t>
+          <t>SPY230629C00443000</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="E24" t="n">
-        <v>0.36</v>
+        <v>0.02</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>-66.66667</v>
       </c>
       <c r="J24" t="n">
-        <v>5122</v>
+        <v>3613</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>3059</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0312596875</v>
+        <v>0.104501142578125</v>
       </c>
       <c r="M24" t="b">
         <v>0</v>
@@ -2084,22 +2104,22 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>-0.005</v>
       </c>
       <c r="U24" t="n">
-        <v>0</v>
+        <v>266579.4900268555</v>
       </c>
     </row>
     <row r="25">
@@ -2108,36 +2128,36 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SPY230628C00439000</t>
+          <t>SPY230629C00444000</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="E25" t="n">
-        <v>0.23</v>
+        <v>0.02</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="J25" t="n">
-        <v>4768</v>
+        <v>4028</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>2043</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0312596875</v>
+        <v>0.117196328125</v>
       </c>
       <c r="M25" t="b">
         <v>0</v>
@@ -2153,22 +2173,22 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
       </c>
       <c r="T25" t="n">
-        <v>0</v>
+        <v>-0.005</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>89019.59760131837</v>
       </c>
     </row>
     <row r="26">
@@ -2177,36 +2197,36 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SPY230628C00440000</t>
+          <t>SPY230629C00445000</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="E26" t="n">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>-33.333336</v>
       </c>
       <c r="J26" t="n">
-        <v>7706</v>
+        <v>1490</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>2163</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0312596875</v>
+        <v>0.1289149609375</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
@@ -2222,22 +2242,22 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
       </c>
       <c r="T26" t="n">
-        <v>0</v>
+        <v>-0.005</v>
       </c>
       <c r="U26" t="n">
-        <v>0</v>
+        <v>94248.35516967774</v>
       </c>
     </row>
     <row r="27">
@@ -2246,36 +2266,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SPY230628C00441000</t>
+          <t>SPY230629C00446000</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="E27" t="n">
-        <v>0.08</v>
+        <v>0.01</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="J27" t="n">
-        <v>2574</v>
+        <v>543</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>1145</v>
       </c>
       <c r="L27" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.1289149609375</v>
       </c>
       <c r="M27" t="b">
         <v>0</v>
@@ -2303,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>-0.002</v>
       </c>
       <c r="U27" t="n">
         <v>0</v>
@@ -2315,21 +2335,21 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SPY230628C00442000</t>
+          <t>SPY230629C00447000</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="E28" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -2338,13 +2358,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1305</v>
+        <v>3514</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>2761</v>
       </c>
       <c r="L28" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.14063359375</v>
       </c>
       <c r="M28" t="b">
         <v>0</v>
@@ -2372,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="T28" t="n">
-        <v>0</v>
+        <v>-0.002</v>
       </c>
       <c r="U28" t="n">
         <v>0</v>
@@ -2384,21 +2404,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SPY230628C00443000</t>
+          <t>SPY230629C00448000</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="n">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="E29" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -2407,13 +2427,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>964</v>
+        <v>1467</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1308</v>
       </c>
       <c r="L29" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.15039912109375</v>
       </c>
       <c r="M29" t="b">
         <v>0</v>
@@ -2441,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U29" t="n">
         <v>0</v>
@@ -2453,21 +2473,21 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SPY230628C00444000</t>
+          <t>SPY230629C00450000</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="E30" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2476,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>457</v>
+        <v>68</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>2122</v>
       </c>
       <c r="L30" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.17188328125</v>
       </c>
       <c r="M30" t="b">
         <v>0</v>
@@ -2510,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="T30" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U30" t="n">
         <v>0</v>
@@ -2522,21 +2542,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SPY230628C00445000</t>
+          <t>SPY230629C00452000</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2545,13 +2565,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1180</v>
+        <v>4</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L31" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.1914143359375</v>
       </c>
       <c r="M31" t="b">
         <v>0</v>
@@ -2579,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U31" t="n">
         <v>0</v>
@@ -2591,21 +2611,21 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SPY230628C00446000</t>
+          <t>SPY230629C00454000</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E32" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -2614,13 +2634,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>2021</v>
       </c>
       <c r="L32" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.210945390625</v>
       </c>
       <c r="M32" t="b">
         <v>0</v>
@@ -2648,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U32" t="n">
         <v>0</v>
@@ -2660,12 +2680,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SPY230628C00448000</t>
+          <t>SPY230629C00456000</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="E33" t="n">
         <v>0.01</v>
@@ -2674,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2683,13 +2703,13 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>1044</v>
+        <v>5</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="L33" t="n">
-        <v>0.06250937500000001</v>
+        <v>0.23438265625</v>
       </c>
       <c r="M33" t="b">
         <v>0</v>
@@ -2717,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U33" t="n">
         <v>0</v>
@@ -2729,12 +2749,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SPY230628C00450000</t>
+          <t>SPY230629C00458000</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="E34" t="n">
         <v>0.01</v>
@@ -2743,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -2752,13 +2772,13 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>395</v>
+        <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="L34" t="n">
-        <v>0.12500875</v>
+        <v>0.2539137109375</v>
       </c>
       <c r="M34" t="b">
         <v>0</v>
@@ -2786,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U34" t="n">
         <v>0</v>
@@ -2798,12 +2818,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SPY230628C00452000</t>
+          <t>SPY230629C00460000</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="E35" t="n">
         <v>0.01</v>
@@ -2812,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -2821,13 +2841,13 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>825</v>
+        <v>100</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>1527</v>
       </c>
       <c r="L35" t="n">
-        <v>0.12500875</v>
+        <v>0.273444765625</v>
       </c>
       <c r="M35" t="b">
         <v>0</v>
@@ -2855,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="T35" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U35" t="n">
         <v>0</v>
@@ -2867,12 +2887,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SPY230628C00454000</t>
+          <t>SPY230629C00470000</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>454</v>
+        <v>470</v>
       </c>
       <c r="E36" t="n">
         <v>0.01</v>
@@ -2881,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -2890,13 +2910,13 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="L36" t="n">
-        <v>0.12500875</v>
+        <v>0.367193828125</v>
       </c>
       <c r="M36" t="b">
         <v>0</v>
@@ -2924,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U36" t="n">
         <v>0</v>
@@ -2936,12 +2956,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SPY230628C00456000</t>
+          <t>SPY230629C00480000</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>456</v>
+        <v>480</v>
       </c>
       <c r="E37" t="n">
         <v>0.01</v>
@@ -2950,7 +2970,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -2959,13 +2979,13 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="L37" t="n">
-        <v>0.12500875</v>
+        <v>0.460942890625</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>
@@ -2993,561 +3013,9 @@
         <v>0</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>SPY230628C00458000</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="n">
-        <v>458</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>2</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0.12500875</v>
-      </c>
-      <c r="M38" t="b">
-        <v>0</v>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="n">
-        <v>0</v>
-      </c>
-      <c r="S38" t="n">
-        <v>0</v>
-      </c>
-      <c r="T38" t="n">
-        <v>0</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>SPY230628C00460000</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="n">
-        <v>460</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" t="n">
-        <v>215</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0.12500875</v>
-      </c>
-      <c r="M39" t="b">
-        <v>0</v>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="n">
-        <v>0</v>
-      </c>
-      <c r="S39" t="n">
-        <v>0</v>
-      </c>
-      <c r="T39" t="n">
-        <v>0</v>
-      </c>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>SPY230628C00462000</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="n">
-        <v>462</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" t="n">
-        <v>3</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0.12500875</v>
-      </c>
-      <c r="M40" t="b">
-        <v>0</v>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" t="n">
-        <v>0</v>
-      </c>
-      <c r="S40" t="n">
-        <v>0</v>
-      </c>
-      <c r="T40" t="n">
-        <v>0</v>
-      </c>
-      <c r="U40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>SPY230628C00464000</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="n">
-        <v>464</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>75</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0.12500875</v>
-      </c>
-      <c r="M41" t="b">
-        <v>0</v>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="n">
-        <v>0</v>
-      </c>
-      <c r="S41" t="n">
-        <v>0</v>
-      </c>
-      <c r="T41" t="n">
-        <v>0</v>
-      </c>
-      <c r="U41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>SPY230628C00466000</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="n">
-        <v>466</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>2</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0.12500875</v>
-      </c>
-      <c r="M42" t="b">
-        <v>0</v>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="n">
-        <v>0</v>
-      </c>
-      <c r="S42" t="n">
-        <v>0</v>
-      </c>
-      <c r="T42" t="n">
-        <v>0</v>
-      </c>
-      <c r="U42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>SPY230628C00468000</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="n">
-        <v>468</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" t="n">
-        <v>27</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0.2500075</v>
-      </c>
-      <c r="M43" t="b">
-        <v>0</v>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="n">
-        <v>0</v>
-      </c>
-      <c r="S43" t="n">
-        <v>0</v>
-      </c>
-      <c r="T43" t="n">
-        <v>0</v>
-      </c>
-      <c r="U43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>SPY230628C00470000</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="n">
-        <v>470</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>23</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0.2500075</v>
-      </c>
-      <c r="M44" t="b">
-        <v>0</v>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" t="n">
-        <v>0</v>
-      </c>
-      <c r="S44" t="n">
-        <v>0</v>
-      </c>
-      <c r="T44" t="n">
-        <v>0</v>
-      </c>
-      <c r="U44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>SPY230628C00480000</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="n">
-        <v>480</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>1</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0.2500075</v>
-      </c>
-      <c r="M45" t="b">
-        <v>0</v>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="P45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" t="n">
-        <v>0</v>
-      </c>
-      <c r="S45" t="n">
-        <v>0</v>
-      </c>
-      <c r="T45" t="n">
-        <v>0</v>
-      </c>
-      <c r="U45" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ready to test task scheduler
</commit_message>
<xml_diff>
--- a/calls_dol_gammas.xlsx
+++ b/calls_dol_gammas.xlsx
@@ -552,10 +552,10 @@
         <v>55.9</v>
       </c>
       <c r="F2" t="n">
-        <v>55.29</v>
+        <v>56.33</v>
       </c>
       <c r="G2" t="n">
-        <v>55.54</v>
+        <v>57.36</v>
       </c>
       <c r="H2" t="n">
         <v>2.3199997</v>
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
-        <v>1e-05</v>
+        <v>1.041996977539063</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -586,22 +586,22 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.995</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="S2" t="n">
         <v>0.01</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.055</v>
+        <v>-0.23</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>698.2240234375</v>
       </c>
     </row>
     <row r="3">
@@ -621,16 +621,16 @@
         <v>44.91</v>
       </c>
       <c r="F3" t="n">
-        <v>45.3</v>
+        <v>46.45</v>
       </c>
       <c r="G3" t="n">
-        <v>45.55</v>
+        <v>47.28</v>
       </c>
       <c r="H3" t="n">
         <v>-1.7999992</v>
       </c>
       <c r="I3" t="n">
-        <v>-3.853563</v>
+        <v>-3.8535628</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -639,7 +639,7 @@
         <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>1e-05</v>
+        <v>0.88476677734375</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -655,22 +655,22 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="S3" t="n">
         <v>0.011</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.056</v>
+        <v>-0.255</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>130.9170043945312</v>
       </c>
     </row>
     <row r="4">
@@ -687,28 +687,28 @@
         <v>400</v>
       </c>
       <c r="E4" t="n">
-        <v>35.67</v>
+        <v>36</v>
       </c>
       <c r="F4" t="n">
-        <v>35.26</v>
+        <v>36.5</v>
       </c>
       <c r="G4" t="n">
-        <v>35.55</v>
+        <v>37.32</v>
       </c>
       <c r="H4" t="n">
-        <v>3.709999</v>
+        <v>4.040001</v>
       </c>
       <c r="I4" t="n">
-        <v>11.608258</v>
+        <v>12.640804</v>
       </c>
       <c r="J4" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K4" t="n">
         <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>1e-05</v>
+        <v>0.7324245507812499</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
+        <v>0.989</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
       <c r="S4" t="n">
         <v>0.011</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.058</v>
+        <v>-0.297</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>174.556005859375</v>
       </c>
     </row>
     <row r="5">
@@ -759,16 +759,16 @@
         <v>25.59</v>
       </c>
       <c r="F5" t="n">
-        <v>25.3</v>
+        <v>26.46</v>
       </c>
       <c r="G5" t="n">
-        <v>25.55</v>
+        <v>27.29</v>
       </c>
       <c r="H5" t="n">
         <v>2.8099995</v>
       </c>
       <c r="I5" t="n">
-        <v>12.335379</v>
+        <v>12.33538</v>
       </c>
       <c r="J5" t="n">
         <v>12</v>
@@ -777,7 +777,7 @@
         <v>17</v>
       </c>
       <c r="L5" t="n">
-        <v>1e-05</v>
+        <v>0.5542036767578126</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -793,22 +793,22 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>0.985</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="S5" t="n">
         <v>0.011</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.059</v>
+        <v>-0.298</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>2225.589074707032</v>
       </c>
     </row>
     <row r="6">
@@ -828,16 +828,16 @@
         <v>15.85</v>
       </c>
       <c r="F6" t="n">
-        <v>15.39</v>
+        <v>16.51</v>
       </c>
       <c r="G6" t="n">
-        <v>15.65</v>
+        <v>17.34</v>
       </c>
       <c r="H6" t="n">
         <v>-0.6900005299999999</v>
       </c>
       <c r="I6" t="n">
-        <v>-4.171708</v>
+        <v>-4.1717076</v>
       </c>
       <c r="J6" t="n">
         <v>155</v>
@@ -846,7 +846,7 @@
         <v>66</v>
       </c>
       <c r="L6" t="n">
-        <v>1e-05</v>
+        <v>0.4594780615234375</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -862,22 +862,22 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>0.946</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="S6" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.06</v>
+        <v>-0.63</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>28801.74096679688</v>
       </c>
     </row>
     <row r="7">
@@ -894,28 +894,28 @@
         <v>424</v>
       </c>
       <c r="E7" t="n">
-        <v>11.75</v>
+        <v>11.64</v>
       </c>
       <c r="F7" t="n">
-        <v>11.34</v>
+        <v>12.63</v>
       </c>
       <c r="G7" t="n">
-        <v>11.56</v>
+        <v>13.23</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.0299997</v>
+        <v>-1.1399994</v>
       </c>
       <c r="I7" t="n">
-        <v>-8.059464999999999</v>
+        <v>-8.920183</v>
       </c>
       <c r="J7" t="n">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K7" t="n">
         <v>49</v>
       </c>
       <c r="L7" t="n">
-        <v>1e-05</v>
+        <v>0.3632876171875</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -931,22 +931,22 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.015</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
       <c r="S7" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.061</v>
+        <v>-0.569</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>32074.66607666016</v>
       </c>
     </row>
     <row r="8">
@@ -963,28 +963,28 @@
         <v>426</v>
       </c>
       <c r="E8" t="n">
-        <v>9.539999999999999</v>
+        <v>10.88</v>
       </c>
       <c r="F8" t="n">
-        <v>9.42</v>
+        <v>10.64</v>
       </c>
       <c r="G8" t="n">
-        <v>9.65</v>
+        <v>11.24</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.75</v>
+        <v>0.5900001499999999</v>
       </c>
       <c r="I8" t="n">
-        <v>-7.2886295</v>
+        <v>5.7337236</v>
       </c>
       <c r="J8" t="n">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="K8" t="n">
         <v>20</v>
       </c>
       <c r="L8" t="n">
-        <v>1e-05</v>
+        <v>0.3234930932617187</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1000,22 +1000,22 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>0.019</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
       <c r="S8" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.061</v>
+        <v>-0.579</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>16582.82055664062</v>
       </c>
     </row>
     <row r="9">
@@ -1032,28 +1032,28 @@
         <v>428</v>
       </c>
       <c r="E9" t="n">
-        <v>7.61</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>7.35</v>
+        <v>8.65</v>
       </c>
       <c r="G9" t="n">
-        <v>7.57</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.3200002</v>
+        <v>0.03999996</v>
       </c>
       <c r="I9" t="n">
-        <v>-14.781636</v>
+        <v>0.4479279</v>
       </c>
       <c r="J9" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K9" t="n">
         <v>66</v>
       </c>
       <c r="L9" t="n">
-        <v>1e-05</v>
+        <v>0.2504957763671875</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>
@@ -1069,22 +1069,22 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="S9" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.062</v>
+        <v>-0.429</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>66244.00422363282</v>
       </c>
     </row>
     <row r="10">
@@ -1101,28 +1101,28 @@
         <v>429</v>
       </c>
       <c r="E10" t="n">
-        <v>6.48</v>
+        <v>7.5</v>
       </c>
       <c r="F10" t="n">
-        <v>6.37</v>
+        <v>7.65</v>
       </c>
       <c r="G10" t="n">
-        <v>6.61</v>
+        <v>8.24</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.75</v>
+        <v>0.26999998</v>
       </c>
       <c r="I10" t="n">
-        <v>-10.373444</v>
+        <v>3.7344396</v>
       </c>
       <c r="J10" t="n">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="K10" t="n">
         <v>122</v>
       </c>
       <c r="L10" t="n">
-        <v>1e-05</v>
+        <v>0.2592847509765626</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -1138,22 +1138,22 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>1</v>
+        <v>0.899</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="S10" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.062</v>
+        <v>-0.579</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>159718.7453613281</v>
       </c>
     </row>
     <row r="11">
@@ -1170,28 +1170,28 @@
         <v>430</v>
       </c>
       <c r="E11" t="n">
-        <v>5.59</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>5.39</v>
+        <v>6.66</v>
       </c>
       <c r="G11" t="n">
-        <v>5.6</v>
+        <v>7.1</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.7100000400000001</v>
+        <v>0.6999997999999999</v>
       </c>
       <c r="I11" t="n">
-        <v>-11.269841</v>
+        <v>11.111108</v>
       </c>
       <c r="J11" t="n">
-        <v>434</v>
+        <v>550</v>
       </c>
       <c r="K11" t="n">
         <v>894</v>
       </c>
       <c r="L11" t="n">
-        <v>1e-05</v>
+        <v>0.2209550561523437</v>
       </c>
       <c r="M11" t="b">
         <v>1</v>
@@ -1207,22 +1207,22 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>1</v>
+        <v>0.902</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="S11" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.062</v>
+        <v>-0.492</v>
       </c>
       <c r="U11" t="n">
-        <v>0</v>
+        <v>1326451.08852539</v>
       </c>
     </row>
     <row r="12">
@@ -1239,28 +1239,28 @@
         <v>431</v>
       </c>
       <c r="E12" t="n">
-        <v>4.54</v>
+        <v>5.96</v>
       </c>
       <c r="F12" t="n">
-        <v>4.36</v>
+        <v>5.68</v>
       </c>
       <c r="G12" t="n">
-        <v>4.59</v>
+        <v>6.26</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.5100002</v>
+        <v>-0.09000015</v>
       </c>
       <c r="I12" t="n">
-        <v>-24.958681</v>
+        <v>-1.4876057</v>
       </c>
       <c r="J12" t="n">
-        <v>1102</v>
+        <v>1139</v>
       </c>
       <c r="K12" t="n">
         <v>2429</v>
       </c>
       <c r="L12" t="n">
-        <v>1e-05</v>
+        <v>0.2163164306640625</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1276,22 +1276,22 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>1</v>
+        <v>0.868</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>0.049</v>
       </c>
       <c r="S12" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.062</v>
+        <v>-0.582</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>4557962.785998534</v>
       </c>
     </row>
     <row r="13">
@@ -1308,28 +1308,28 @@
         <v>432</v>
       </c>
       <c r="E13" t="n">
-        <v>3.65</v>
+        <v>4.91</v>
       </c>
       <c r="F13" t="n">
-        <v>3.48</v>
+        <v>4.71</v>
       </c>
       <c r="G13" t="n">
-        <v>3.64</v>
+        <v>5.12</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.7999997</v>
+        <v>0.46000004</v>
       </c>
       <c r="I13" t="n">
-        <v>-17.977522</v>
+        <v>10.33708</v>
       </c>
       <c r="J13" t="n">
-        <v>1185</v>
+        <v>1329</v>
       </c>
       <c r="K13" t="n">
         <v>2962</v>
       </c>
       <c r="L13" t="n">
-        <v>1e-05</v>
+        <v>0.1782308740234375</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1345,22 +1345,22 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>1</v>
+        <v>0.865</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>0.053</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="S13" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.062</v>
+        <v>-0.495</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>6850712.283959961</v>
       </c>
     </row>
     <row r="14">
@@ -1377,28 +1377,28 @@
         <v>433</v>
       </c>
       <c r="E14" t="n">
-        <v>2.78</v>
+        <v>4.1</v>
       </c>
       <c r="F14" t="n">
-        <v>2.68</v>
+        <v>3.78</v>
       </c>
       <c r="G14" t="n">
-        <v>2.71</v>
+        <v>4.32</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.77</v>
+        <v>0.54999995</v>
       </c>
       <c r="I14" t="n">
-        <v>-21.690142</v>
+        <v>15.492956</v>
       </c>
       <c r="J14" t="n">
-        <v>5659</v>
+        <v>6228</v>
       </c>
       <c r="K14" t="n">
         <v>3625</v>
       </c>
       <c r="L14" t="n">
-        <v>1e-05</v>
+        <v>0.1733481103515625</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
@@ -1414,22 +1414,22 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>1</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>0.062</v>
       </c>
       <c r="S14" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.062</v>
+        <v>-0.587</v>
       </c>
       <c r="U14" t="n">
-        <v>0</v>
+        <v>10757013.86108399</v>
       </c>
     </row>
     <row r="15">
@@ -1446,28 +1446,28 @@
         <v>434</v>
       </c>
       <c r="E15" t="n">
-        <v>2.03</v>
+        <v>3.1</v>
       </c>
       <c r="F15" t="n">
-        <v>1.97</v>
+        <v>2.91</v>
       </c>
       <c r="G15" t="n">
-        <v>1.99</v>
+        <v>3.4</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.77</v>
+        <v>0.29999995</v>
       </c>
       <c r="I15" t="n">
-        <v>-27.5</v>
+        <v>10.714284</v>
       </c>
       <c r="J15" t="n">
-        <v>24408</v>
+        <v>26316</v>
       </c>
       <c r="K15" t="n">
         <v>4854</v>
       </c>
       <c r="L15" t="n">
-        <v>0.06714800048828126</v>
+        <v>0.1540611938476563</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
@@ -1483,22 +1483,22 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>0.878</v>
+        <v>0.759</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.132</v>
+        <v>0.089</v>
       </c>
       <c r="R15" t="n">
-        <v>0.046</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="S15" t="n">
-        <v>0.01</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.21</v>
+        <v>-0.596</v>
       </c>
       <c r="U15" t="n">
-        <v>27918428.16049805</v>
+        <v>18852310.46682129</v>
       </c>
     </row>
     <row r="16">
@@ -1515,28 +1515,28 @@
         <v>435</v>
       </c>
       <c r="E16" t="n">
-        <v>1.42</v>
+        <v>2.35</v>
       </c>
       <c r="F16" t="n">
-        <v>1.39</v>
+        <v>2.34</v>
       </c>
       <c r="G16" t="n">
-        <v>1.4</v>
+        <v>2.37</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.7200001499999999</v>
+        <v>0.2099998</v>
       </c>
       <c r="I16" t="n">
-        <v>-33.644863</v>
+        <v>9.813074</v>
       </c>
       <c r="J16" t="n">
-        <v>101637</v>
+        <v>111058</v>
       </c>
       <c r="K16" t="n">
         <v>7759</v>
       </c>
       <c r="L16" t="n">
-        <v>0.07715766601562501</v>
+        <v>0.1226894372558594</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -1552,22 +1552,22 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>0.672</v>
+        <v>0.699</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.205</v>
+        <v>0.124</v>
       </c>
       <c r="R16" t="n">
-        <v>0.082</v>
+        <v>0.08</v>
       </c>
       <c r="S16" t="n">
         <v>0.008</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.36</v>
+        <v>-0.531</v>
       </c>
       <c r="U16" t="n">
-        <v>69306963.70370482</v>
+        <v>41985781.53334961</v>
       </c>
     </row>
     <row r="17">
@@ -1584,31 +1584,31 @@
         <v>436</v>
       </c>
       <c r="E17" t="n">
-        <v>0.91</v>
+        <v>1.65</v>
       </c>
       <c r="F17" t="n">
-        <v>0.89</v>
+        <v>1.65</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9</v>
+        <v>1.67</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.6499999</v>
+        <v>0.09000002999999999</v>
       </c>
       <c r="I17" t="n">
-        <v>-41.666664</v>
+        <v>5.769233</v>
       </c>
       <c r="J17" t="n">
-        <v>199597</v>
+        <v>222975</v>
       </c>
       <c r="K17" t="n">
         <v>7028</v>
       </c>
       <c r="L17" t="n">
-        <v>0.07996525512695313</v>
+        <v>0.1139004626464844</v>
       </c>
       <c r="M17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -1621,22 +1621,22 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>0.452</v>
+        <v>0.57</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.217</v>
+        <v>0.151</v>
       </c>
       <c r="R17" t="n">
         <v>0.09</v>
       </c>
       <c r="S17" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.389</v>
+        <v>-0.546</v>
       </c>
       <c r="U17" t="n">
-        <v>66452105.64436036</v>
+        <v>46310930.24653321</v>
       </c>
     </row>
     <row r="18">
@@ -1653,28 +1653,28 @@
         <v>437</v>
       </c>
       <c r="E18" t="n">
-        <v>0.54</v>
+        <v>1.08</v>
       </c>
       <c r="F18" t="n">
-        <v>0.52</v>
+        <v>1.08</v>
       </c>
       <c r="G18" t="n">
-        <v>0.53</v>
+        <v>1.09</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.57</v>
+        <v>-0.029999971</v>
       </c>
       <c r="I18" t="n">
-        <v>-51.35135</v>
+        <v>-2.7027001</v>
       </c>
       <c r="J18" t="n">
-        <v>134524</v>
+        <v>149039</v>
       </c>
       <c r="K18" t="n">
         <v>4017</v>
       </c>
       <c r="L18" t="n">
-        <v>0.081063876953125</v>
+        <v>0.106454248046875</v>
       </c>
       <c r="M18" t="b">
         <v>0</v>
@@ -1690,22 +1690,22 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>0.255</v>
+        <v>0.412</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.174</v>
+        <v>0.16</v>
       </c>
       <c r="R18" t="n">
-        <v>0.073</v>
+        <v>0.089</v>
       </c>
       <c r="S18" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.313</v>
+        <v>-0.499</v>
       </c>
       <c r="U18" t="n">
-        <v>30455682.77054444</v>
+        <v>28047659.02148438</v>
       </c>
     </row>
     <row r="19">
@@ -1722,28 +1722,28 @@
         <v>438</v>
       </c>
       <c r="E19" t="n">
-        <v>0.29</v>
+        <v>0.66</v>
       </c>
       <c r="F19" t="n">
-        <v>0.29</v>
+        <v>0.65</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3</v>
+        <v>0.66</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.45000002</v>
+        <v>-0.07999998</v>
       </c>
       <c r="I19" t="n">
-        <v>-60.81081</v>
+        <v>-10.810808</v>
       </c>
       <c r="J19" t="n">
-        <v>63264</v>
+        <v>74595</v>
       </c>
       <c r="K19" t="n">
         <v>4199</v>
       </c>
       <c r="L19" t="n">
-        <v>0.08326112060546878</v>
+        <v>0.101571484375</v>
       </c>
       <c r="M19" t="b">
         <v>0</v>
@@ -1759,22 +1759,22 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>0.122</v>
+        <v>0.254</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.107</v>
+        <v>0.138</v>
       </c>
       <c r="R19" t="n">
-        <v>0.046</v>
+        <v>0.073</v>
       </c>
       <c r="S19" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.2</v>
+        <v>-0.387</v>
       </c>
       <c r="U19" t="n">
-        <v>19577034.78467407</v>
+        <v>25287143.0668213</v>
       </c>
     </row>
     <row r="20">
@@ -1791,28 +1791,28 @@
         <v>439</v>
       </c>
       <c r="E20" t="n">
-        <v>0.16</v>
+        <v>0.36</v>
       </c>
       <c r="F20" t="n">
-        <v>0.14</v>
+        <v>0.36</v>
       </c>
       <c r="G20" t="n">
-        <v>0.15</v>
+        <v>0.37</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.34</v>
+        <v>-0.13999999</v>
       </c>
       <c r="I20" t="n">
-        <v>-68</v>
+        <v>-27.999996</v>
       </c>
       <c r="J20" t="n">
-        <v>51433</v>
+        <v>73105</v>
       </c>
       <c r="K20" t="n">
         <v>2929</v>
       </c>
       <c r="L20" t="n">
-        <v>0.08374939697265626</v>
+        <v>0.09839768798828125</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
@@ -1828,22 +1828,22 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>0.047</v>
+        <v>0.13</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.051</v>
+        <v>0.094</v>
       </c>
       <c r="R20" t="n">
-        <v>0.022</v>
+        <v>0.048</v>
       </c>
       <c r="S20" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.096</v>
+        <v>-0.246</v>
       </c>
       <c r="U20" t="n">
-        <v>6508888.140032959</v>
+        <v>12014951.71730957</v>
       </c>
     </row>
     <row r="21">
@@ -1860,28 +1860,28 @@
         <v>440</v>
       </c>
       <c r="E21" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="F21" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="G21" t="n">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.23</v>
+        <v>-0.13</v>
       </c>
       <c r="I21" t="n">
-        <v>-74.19355</v>
+        <v>-41.935482</v>
       </c>
       <c r="J21" t="n">
-        <v>75854</v>
+        <v>109121</v>
       </c>
       <c r="K21" t="n">
         <v>8585</v>
       </c>
       <c r="L21" t="n">
-        <v>0.08692319335937501</v>
+        <v>0.09449147705078126</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -1897,22 +1897,22 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>0.017</v>
+        <v>0.051</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.021</v>
+        <v>0.049</v>
       </c>
       <c r="R21" t="n">
-        <v>0.01</v>
+        <v>0.024</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.043</v>
+        <v>-0.116</v>
       </c>
       <c r="U21" t="n">
-        <v>7855554.651763918</v>
+        <v>18357400.5512085</v>
       </c>
     </row>
     <row r="22">
@@ -1929,28 +1929,28 @@
         <v>441</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="F22" t="n">
-        <v>0.04</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G22" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.13000001</v>
+        <v>-0.10000001</v>
       </c>
       <c r="I22" t="n">
-        <v>-72.22223</v>
+        <v>-55.555557</v>
       </c>
       <c r="J22" t="n">
-        <v>23319</v>
+        <v>27477</v>
       </c>
       <c r="K22" t="n">
         <v>2061</v>
       </c>
       <c r="L22" t="n">
-        <v>0.09327078613281251</v>
+        <v>0.09229423339843749</v>
       </c>
       <c r="M22" t="b">
         <v>0</v>
@@ -1966,22 +1966,22 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>0.007</v>
+        <v>0.016</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.01</v>
+        <v>0.019</v>
       </c>
       <c r="R22" t="n">
-        <v>0.005</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.022</v>
+        <v>-0.043</v>
       </c>
       <c r="U22" t="n">
-        <v>898039.1123657227</v>
+        <v>1708859.658361817</v>
       </c>
     </row>
     <row r="23">
@@ -1998,28 +1998,28 @@
         <v>442</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="F23" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G23" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.09</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I23" t="n">
-        <v>-81.818184</v>
+        <v>-63.636364</v>
       </c>
       <c r="J23" t="n">
-        <v>9819</v>
+        <v>10862</v>
       </c>
       <c r="K23" t="n">
         <v>3510</v>
       </c>
       <c r="L23" t="n">
-        <v>0.098641826171875</v>
+        <v>0.0937590625</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -2035,22 +2035,22 @@
         </is>
       </c>
       <c r="P23" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="R23" t="n">
         <v>0.003</v>
       </c>
-      <c r="Q23" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0.002</v>
-      </c>
       <c r="S23" t="n">
         <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>-0.011</v>
+        <v>-0.016</v>
       </c>
       <c r="U23" t="n">
-        <v>611764.6354980469</v>
+        <v>1072210.265991211</v>
       </c>
     </row>
     <row r="24">
@@ -2082,13 +2082,13 @@
         <v>-66.66667</v>
       </c>
       <c r="J24" t="n">
-        <v>3613</v>
+        <v>4123</v>
       </c>
       <c r="K24" t="n">
         <v>3059</v>
       </c>
       <c r="L24" t="n">
-        <v>0.104501142578125</v>
+        <v>0.09668872070312501</v>
       </c>
       <c r="M24" t="b">
         <v>0</v>
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="Q24" t="n">
         <v>0.002</v>
@@ -2116,10 +2116,10 @@
         <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.005</v>
+        <v>-0.006</v>
       </c>
       <c r="U24" t="n">
-        <v>266579.4900268555</v>
+        <v>266983.4109619141</v>
       </c>
     </row>
     <row r="25">
@@ -2151,13 +2151,13 @@
         <v>-50</v>
       </c>
       <c r="J25" t="n">
-        <v>4028</v>
+        <v>4131</v>
       </c>
       <c r="K25" t="n">
         <v>2043</v>
       </c>
       <c r="L25" t="n">
-        <v>0.117196328125</v>
+        <v>0.10938390625</v>
       </c>
       <c r="M25" t="b">
         <v>0</v>
@@ -2176,7 +2176,7 @@
         <v>0.001</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="R25" t="n">
         <v>0.001</v>
@@ -2185,10 +2185,10 @@
         <v>0</v>
       </c>
       <c r="T25" t="n">
-        <v>-0.005</v>
+        <v>-0.006</v>
       </c>
       <c r="U25" t="n">
-        <v>89019.59760131837</v>
+        <v>178308.9599853516</v>
       </c>
     </row>
     <row r="26">
@@ -2205,7 +2205,7 @@
         <v>445</v>
       </c>
       <c r="E26" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F26" t="n">
         <v>0.01</v>
@@ -2214,19 +2214,19 @@
         <v>0.02</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="I26" t="n">
-        <v>-33.333336</v>
+        <v>-66.66667</v>
       </c>
       <c r="J26" t="n">
-        <v>1490</v>
+        <v>1632</v>
       </c>
       <c r="K26" t="n">
         <v>2163</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1289149609375</v>
+        <v>0.1211025390625</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
@@ -2257,7 +2257,7 @@
         <v>-0.005</v>
       </c>
       <c r="U26" t="n">
-        <v>94248.35516967774</v>
+        <v>94391.16016845703</v>
       </c>
     </row>
     <row r="27">
@@ -2289,13 +2289,13 @@
         <v>-50</v>
       </c>
       <c r="J27" t="n">
-        <v>543</v>
+        <v>1288</v>
       </c>
       <c r="K27" t="n">
         <v>1145</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1289149609375</v>
+        <v>0.1211025390625</v>
       </c>
       <c r="M27" t="b">
         <v>0</v>
@@ -2358,13 +2358,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>3514</v>
+        <v>3531</v>
       </c>
       <c r="K28" t="n">
         <v>2761</v>
       </c>
       <c r="L28" t="n">
-        <v>0.14063359375</v>
+        <v>0.132821171875</v>
       </c>
       <c r="M28" t="b">
         <v>0</v>
@@ -2427,13 +2427,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1467</v>
+        <v>1488</v>
       </c>
       <c r="K29" t="n">
         <v>1308</v>
       </c>
       <c r="L29" t="n">
-        <v>0.15039912109375</v>
+        <v>0.1445398046875</v>
       </c>
       <c r="M29" t="b">
         <v>0</v>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="U29" t="n">
         <v>0</v>
@@ -2496,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="K30" t="n">
         <v>2122</v>
       </c>
       <c r="L30" t="n">
-        <v>0.17188328125</v>
+        <v>0.164070859375</v>
       </c>
       <c r="M30" t="b">
         <v>0</v>
@@ -2571,7 +2571,7 @@
         <v>20</v>
       </c>
       <c r="L31" t="n">
-        <v>0.1914143359375</v>
+        <v>0.1836019140625</v>
       </c>
       <c r="M31" t="b">
         <v>0</v>
@@ -2640,7 +2640,7 @@
         <v>2021</v>
       </c>
       <c r="L32" t="n">
-        <v>0.210945390625</v>
+        <v>0.2070391796875</v>
       </c>
       <c r="M32" t="b">
         <v>0</v>
@@ -2709,7 +2709,7 @@
         <v>295</v>
       </c>
       <c r="L33" t="n">
-        <v>0.23438265625</v>
+        <v>0.226570234375</v>
       </c>
       <c r="M33" t="b">
         <v>0</v>
@@ -2778,7 +2778,7 @@
         <v>31</v>
       </c>
       <c r="L34" t="n">
-        <v>0.2539137109375</v>
+        <v>0.2461012890625</v>
       </c>
       <c r="M34" t="b">
         <v>0</v>
@@ -2847,7 +2847,7 @@
         <v>1527</v>
       </c>
       <c r="L35" t="n">
-        <v>0.273444765625</v>
+        <v>0.26563234375</v>
       </c>
       <c r="M35" t="b">
         <v>0</v>
@@ -2916,7 +2916,7 @@
         <v>220</v>
       </c>
       <c r="L36" t="n">
-        <v>0.367193828125</v>
+        <v>0.35938140625</v>
       </c>
       <c r="M36" t="b">
         <v>0</v>
@@ -2985,7 +2985,7 @@
         <v>255</v>
       </c>
       <c r="L37" t="n">
-        <v>0.460942890625</v>
+        <v>0.45313046875</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>

</xml_diff>